<commit_message>
Framework updated on 24th April
</commit_message>
<xml_diff>
--- a/Resources/TestSuit.xlsx
+++ b/Resources/TestSuit.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="165">
   <si>
     <t>TCID</t>
   </si>
@@ -139,9 +139,6 @@
     <t>2018-19</t>
   </si>
   <si>
-    <t>SRNG  Finance Pvt. Ltd.</t>
-  </si>
-  <si>
     <t>imageLMS_xpath</t>
   </si>
   <si>
@@ -206,6 +203,315 @@
   </si>
   <si>
     <t>selectSubLocationId_xpath</t>
+  </si>
+  <si>
+    <t>SRNG Finance Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>feeCollectionChargeType_xpath</t>
+  </si>
+  <si>
+    <t>feeCollectionChargeName_xpath</t>
+  </si>
+  <si>
+    <t>feeCollectionChargeMethod_xpath</t>
+  </si>
+  <si>
+    <t>feeCollectionChargeAmount_xpath</t>
+  </si>
+  <si>
+    <t>feeCollectionAddSymbol_xpath</t>
+  </si>
+  <si>
+    <t>Receivable</t>
+  </si>
+  <si>
+    <t>Document Charges</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>ChargeAmount</t>
+  </si>
+  <si>
+    <t>feeCollectionNextButton_xpath</t>
+  </si>
+  <si>
+    <t>basicForLoanSelect_xpath</t>
+  </si>
+  <si>
+    <t>basicForLoanSelect2_xpath</t>
+  </si>
+  <si>
+    <t>basicForLoanAddress_xpath</t>
+  </si>
+  <si>
+    <t>basicForLoanSaveButton_xpath</t>
+  </si>
+  <si>
+    <t>Income Tax</t>
+  </si>
+  <si>
+    <t>Borrower</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>basisForLoanAddButton_xpath</t>
+  </si>
+  <si>
+    <t>basicForLoanNextButton_xpath</t>
+  </si>
+  <si>
+    <t>createCustomerLink_xpath</t>
+  </si>
+  <si>
+    <t>addCustomerBusinessSaliedSelect_xpath</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>addCustomerFirstName_xpath</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>addCustomerMaritalStatusSelect_xpath</t>
+  </si>
+  <si>
+    <t>MarriageStatus</t>
+  </si>
+  <si>
+    <t>addCustomerDOB_xpath</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>addCustomerQualification_xpath</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>addCustomerIncomeSlab_xpath</t>
+  </si>
+  <si>
+    <t>IncomeSlab</t>
+  </si>
+  <si>
+    <t>addCustomerCategorySelect_xpath</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>BusinessSalied</t>
+  </si>
+  <si>
+    <t>ABCDEFGH</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>03/08/2010</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>segmentIdSelect_xpath</t>
+  </si>
+  <si>
+    <t>SegmentId</t>
+  </si>
+  <si>
+    <t>segmentOccupationSelect_xpath</t>
+  </si>
+  <si>
+    <t>SegmentOccupation</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>kycSegmentAddButton_xpath</t>
+  </si>
+  <si>
+    <t>KycNameSelect_xpath</t>
+  </si>
+  <si>
+    <t>KycNumber_xpath</t>
+  </si>
+  <si>
+    <t>kycDetailsAddButton_xpath</t>
+  </si>
+  <si>
+    <t>KYCName</t>
+  </si>
+  <si>
+    <t>KYCNumber</t>
+  </si>
+  <si>
+    <t>Adharcard No</t>
+  </si>
+  <si>
+    <t>123412341234</t>
+  </si>
+  <si>
+    <t>familyDetailsName_xpath</t>
+  </si>
+  <si>
+    <t>familyDetialsRelationSelect_xpath</t>
+  </si>
+  <si>
+    <t>familyDetialsOccupation_xpath</t>
+  </si>
+  <si>
+    <t>familyDetialsIncome_xpath</t>
+  </si>
+  <si>
+    <t>familyDetialsDOB_xpath</t>
+  </si>
+  <si>
+    <t>familyDetailsAddButton_xpath</t>
+  </si>
+  <si>
+    <t>FamilyDetailsName</t>
+  </si>
+  <si>
+    <t>FamilyDetailsRelation</t>
+  </si>
+  <si>
+    <t>FamilyDetailsOccupation</t>
+  </si>
+  <si>
+    <t>FamilyDetailsIncome</t>
+  </si>
+  <si>
+    <t>FamilyDetailsDOB</t>
+  </si>
+  <si>
+    <t>PQRSFD</t>
+  </si>
+  <si>
+    <t>Wife</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>12/12/1998</t>
+  </si>
+  <si>
+    <t>addAddressButton_xpath</t>
+  </si>
+  <si>
+    <t>addAddressHouseNo_xpath</t>
+  </si>
+  <si>
+    <t>addAddressColony_xpath</t>
+  </si>
+  <si>
+    <t>addAddressCity_xpath</t>
+  </si>
+  <si>
+    <t>addAddressStateSelect_xpath</t>
+  </si>
+  <si>
+    <t>addAddressDistrictIdSelect_xpath</t>
+  </si>
+  <si>
+    <t>addAddressTehsilIdSelect_xpath</t>
+  </si>
+  <si>
+    <t>addAddressPincode_xpath</t>
+  </si>
+  <si>
+    <t>addAddressdistanceFrom_xpath</t>
+  </si>
+  <si>
+    <t>addAddressSaveButton_xpath</t>
+  </si>
+  <si>
+    <t>addAddressCloseButton_xpath</t>
+  </si>
+  <si>
+    <t>AddressHouseNo</t>
+  </si>
+  <si>
+    <t>AddressColony</t>
+  </si>
+  <si>
+    <t>AddressCity</t>
+  </si>
+  <si>
+    <t>AddressState</t>
+  </si>
+  <si>
+    <t>AddressDistrict</t>
+  </si>
+  <si>
+    <t>AddressTehsilID</t>
+  </si>
+  <si>
+    <t>AddressPincode</t>
+  </si>
+  <si>
+    <t>AddressDistanceFrom</t>
+  </si>
+  <si>
+    <t>9-121/A/3</t>
+  </si>
+  <si>
+    <t>ABCDE</t>
+  </si>
+  <si>
+    <t>Hyd</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>addAddressCountry_xpath</t>
+  </si>
+  <si>
+    <t>AddressCountry</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>515151</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>feeCollectionFinalAmt_xpath</t>
+  </si>
+  <si>
+    <t>Anantapur</t>
+  </si>
+  <si>
+    <t>Agali</t>
   </si>
 </sst>
 </file>
@@ -308,7 +614,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -335,6 +641,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -683,10 +990,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -964,7 +1271,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="9"/>
     </row>
@@ -999,7 +1306,7 @@
         <v>23</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="9"/>
     </row>
@@ -1023,10 +1330,10 @@
         <v>26</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1038,10 +1345,10 @@
         <v>26</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1053,10 +1360,10 @@
         <v>18</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1068,10 +1375,10 @@
         <v>18</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1083,10 +1390,10 @@
         <v>18</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1098,24 +1405,735 @@
         <v>26</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1">
       <c r="A31" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="9"/>
+      <c r="D32" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="2" customFormat="1">
+      <c r="A40" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1">
+      <c r="A46" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" t="s">
+        <v>84</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="9"/>
+      <c r="C53" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>88</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="9"/>
+      <c r="C55" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="9"/>
+      <c r="C56" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" t="s">
+        <v>94</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" t="s">
+        <v>96</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="2" customFormat="1">
+      <c r="A58" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" t="s">
+        <v>105</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" t="s">
+        <v>107</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" s="9"/>
+      <c r="C61" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="2" customFormat="1">
+      <c r="A62" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="9"/>
+      <c r="C63" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" t="s">
+        <v>111</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" s="9"/>
+      <c r="C64" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" t="s">
+        <v>112</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="9"/>
+      <c r="C65" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="9"/>
+      <c r="C67" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
+        <v>118</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" s="9"/>
+      <c r="C68" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" t="s">
+        <v>119</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" s="9"/>
+      <c r="C69" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" t="s">
+        <v>120</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="9"/>
+      <c r="C70" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" t="s">
+        <v>121</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="9"/>
+      <c r="C71" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" t="s">
+        <v>122</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="9"/>
+      <c r="C72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B73" s="9"/>
+      <c r="C73" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="2" customFormat="1">
+      <c r="A74" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74" s="9"/>
+      <c r="C74" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75" s="9"/>
+      <c r="C75" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" t="s">
+        <v>135</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76" s="9"/>
+      <c r="C76" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" t="s">
+        <v>136</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B77" s="9"/>
+      <c r="C77" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D77" t="s">
+        <v>137</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B78" s="9"/>
+      <c r="C78" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" t="s">
+        <v>138</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B79" s="9"/>
+      <c r="C79" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D79" t="s">
+        <v>139</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B80" s="9"/>
+      <c r="C80" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D80" t="s">
+        <v>140</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B81" s="9"/>
+      <c r="C81" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" t="s">
+        <v>141</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82" s="9"/>
+      <c r="C82" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" t="s">
+        <v>142</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83" s="9"/>
+      <c r="C83" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D83" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84" s="9"/>
+      <c r="C84" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D84" t="s">
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1125,10 +2143,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AR7" sqref="AR7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1474,7 +2492,7 @@
     <col min="409" max="409" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:46">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -1482,7 +2500,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:46">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1494,7 +2512,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:46">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1506,12 +2524,12 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:46">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:46" ht="30">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1534,28 +2552,124 @@
         <v>33</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM6" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="AN6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AO6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AP6" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AQ6" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AR6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="AT6" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" ht="30">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1569,7 +2683,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>38</v>
@@ -1578,25 +2692,121 @@
         <v>39</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="K7" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="L7" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="N7" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="12" t="s">
-        <v>61</v>
+      <c r="O7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF7" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG7" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI7" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ7" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK7" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL7" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="AM7" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AN7" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="AO7" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AP7" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="AQ7" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR7" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS7" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT7" s="12" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>